<commit_message>
start graphing data with bokeh
</commit_message>
<xml_diff>
--- a/TheInformation_DataStoryteller_02222016.xlsx
+++ b/TheInformation_DataStoryteller_02222016.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Desktop/Information/Recruiting/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26929"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23420" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="IPO Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Ridesharing Data" sheetId="2" r:id="rId2"/>
+    <sheet name="IPO Data (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="IPO Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Ridesharing Data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Year</t>
   </si>
@@ -86,12 +82,21 @@
   <si>
     <t xml:space="preserve">Lyft </t>
   </si>
+  <si>
+    <t># Profitable</t>
+  </si>
+  <si>
+    <t>Number of Tech &amp; Biotech IPOs</t>
+  </si>
+  <si>
+    <t>Total Number of IPOs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,6 +122,22 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,11 +264,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,8 +372,35 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="8">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -361,6 +415,80 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="139700"/>
+          <a:ext cx="4724400" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>Context: The following dataset outlines the number of IPOs that have taken place</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> and the percentange of those companies that were profitable at the time of IPO from 1980 to 2014. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -434,7 +562,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -551,7 +679,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -586,7 +714,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -763,7 +891,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -771,13 +899,1027 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:I41"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:9">
+      <c r="B5" s="2"/>
+      <c r="C5" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="36"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="6">
+        <v>1980</v>
+      </c>
+      <c r="C7" s="7">
+        <v>25</v>
+      </c>
+      <c r="D7" s="37">
+        <v>22</v>
+      </c>
+      <c r="E7" s="7">
+        <v>46</v>
+      </c>
+      <c r="F7" s="40">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1980</v>
+      </c>
+      <c r="H7" s="43">
+        <f>C7+E7</f>
+        <v>71</v>
+      </c>
+      <c r="I7" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="14">
+        <v>1981</v>
+      </c>
+      <c r="C8" s="15">
+        <v>82</v>
+      </c>
+      <c r="D8" s="38">
+        <v>66.42</v>
+      </c>
+      <c r="E8" s="15">
+        <v>110</v>
+      </c>
+      <c r="F8" s="41">
+        <v>93.5</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1981</v>
+      </c>
+      <c r="H8">
+        <f>C8+E8</f>
+        <v>192</v>
+      </c>
+      <c r="I8" s="15">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="6">
+        <v>1982</v>
+      </c>
+      <c r="C9" s="7">
+        <v>44</v>
+      </c>
+      <c r="D9" s="37">
+        <v>36.08</v>
+      </c>
+      <c r="E9" s="7">
+        <v>33</v>
+      </c>
+      <c r="F9" s="40">
+        <v>26.07</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1982</v>
+      </c>
+      <c r="H9">
+        <f>C9+E9</f>
+        <v>77</v>
+      </c>
+      <c r="I9" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="14">
+        <v>1983</v>
+      </c>
+      <c r="C10" s="15">
+        <v>194</v>
+      </c>
+      <c r="D10" s="38">
+        <v>131.91999999999999</v>
+      </c>
+      <c r="E10" s="15">
+        <v>257</v>
+      </c>
+      <c r="F10" s="41">
+        <v>221.02</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1983</v>
+      </c>
+      <c r="H10">
+        <f>C10+E10</f>
+        <v>451</v>
+      </c>
+      <c r="I10" s="15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="6">
+        <v>1984</v>
+      </c>
+      <c r="C11" s="7">
+        <v>52</v>
+      </c>
+      <c r="D11" s="37">
+        <v>42.12</v>
+      </c>
+      <c r="E11" s="7">
+        <v>121</v>
+      </c>
+      <c r="F11" s="40">
+        <v>101.64</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1984</v>
+      </c>
+      <c r="H11">
+        <f>C11+E11</f>
+        <v>173</v>
+      </c>
+      <c r="I11" s="7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="14">
+        <v>1985</v>
+      </c>
+      <c r="C12" s="15">
+        <v>42</v>
+      </c>
+      <c r="D12" s="38">
+        <v>33.18</v>
+      </c>
+      <c r="E12" s="15">
+        <v>145</v>
+      </c>
+      <c r="F12" s="41">
+        <v>126.15</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1985</v>
+      </c>
+      <c r="H12">
+        <f>C12+E12</f>
+        <v>187</v>
+      </c>
+      <c r="I12" s="15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="6">
+        <v>1986</v>
+      </c>
+      <c r="C13" s="7">
+        <v>102</v>
+      </c>
+      <c r="D13" s="37">
+        <v>65.28</v>
+      </c>
+      <c r="E13" s="7">
+        <v>291</v>
+      </c>
+      <c r="F13" s="40">
+        <v>244.44</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1986</v>
+      </c>
+      <c r="H13">
+        <f>C13+E13</f>
+        <v>393</v>
+      </c>
+      <c r="I13" s="7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="14">
+        <v>1987</v>
+      </c>
+      <c r="C14" s="15">
+        <v>69</v>
+      </c>
+      <c r="D14" s="38">
+        <v>51.75</v>
+      </c>
+      <c r="E14" s="15">
+        <v>216</v>
+      </c>
+      <c r="F14" s="41">
+        <v>183.6</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1987</v>
+      </c>
+      <c r="H14">
+        <f>C14+E14</f>
+        <v>285</v>
+      </c>
+      <c r="I14" s="15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="6">
+        <v>1988</v>
+      </c>
+      <c r="C15" s="7">
+        <v>30</v>
+      </c>
+      <c r="D15" s="37">
+        <v>22.2</v>
+      </c>
+      <c r="E15" s="7">
+        <v>72</v>
+      </c>
+      <c r="F15" s="40">
+        <v>62.64</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1988</v>
+      </c>
+      <c r="H15">
+        <f>C15+E15</f>
+        <v>102</v>
+      </c>
+      <c r="I15" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="14">
+        <v>1989</v>
+      </c>
+      <c r="C16" s="15">
+        <v>39</v>
+      </c>
+      <c r="D16" s="38">
+        <v>26.91</v>
+      </c>
+      <c r="E16" s="15">
+        <v>74</v>
+      </c>
+      <c r="F16" s="41">
+        <v>62.16</v>
+      </c>
+      <c r="G16" s="14">
+        <v>1989</v>
+      </c>
+      <c r="H16">
+        <f>C16+E16</f>
+        <v>113</v>
+      </c>
+      <c r="I16" s="15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="6">
+        <v>1990</v>
+      </c>
+      <c r="C17" s="7">
+        <v>35</v>
+      </c>
+      <c r="D17" s="37">
+        <v>29.05</v>
+      </c>
+      <c r="E17" s="7">
+        <v>75</v>
+      </c>
+      <c r="F17" s="40">
+        <v>65.25</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1990</v>
+      </c>
+      <c r="H17">
+        <f>C17+E17</f>
+        <v>110</v>
+      </c>
+      <c r="I17" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="14">
+        <v>1991</v>
+      </c>
+      <c r="C18" s="15">
+        <v>103</v>
+      </c>
+      <c r="D18" s="38">
+        <v>56.65</v>
+      </c>
+      <c r="E18" s="15">
+        <v>183</v>
+      </c>
+      <c r="F18" s="41">
+        <v>161.04</v>
+      </c>
+      <c r="G18" s="14">
+        <v>1991</v>
+      </c>
+      <c r="H18">
+        <f>C18+E18</f>
+        <v>286</v>
+      </c>
+      <c r="I18" s="15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="6">
+        <v>1992</v>
+      </c>
+      <c r="C19" s="7">
+        <v>146</v>
+      </c>
+      <c r="D19" s="37">
+        <v>78.84</v>
+      </c>
+      <c r="E19" s="7">
+        <v>266</v>
+      </c>
+      <c r="F19" s="40">
+        <v>212.8</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1992</v>
+      </c>
+      <c r="H19">
+        <f>C19+E19</f>
+        <v>412</v>
+      </c>
+      <c r="I19" s="7">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="14">
+        <v>1993</v>
+      </c>
+      <c r="C20" s="15">
+        <v>154</v>
+      </c>
+      <c r="D20" s="38">
+        <v>98.56</v>
+      </c>
+      <c r="E20" s="15">
+        <v>355</v>
+      </c>
+      <c r="F20" s="41">
+        <v>262.7</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1993</v>
+      </c>
+      <c r="H20">
+        <f>C20+E20</f>
+        <v>509</v>
+      </c>
+      <c r="I20" s="15">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="6">
+        <v>1994</v>
+      </c>
+      <c r="C21" s="7">
+        <v>137</v>
+      </c>
+      <c r="D21" s="37">
+        <v>86.31</v>
+      </c>
+      <c r="E21" s="7">
+        <v>266</v>
+      </c>
+      <c r="F21" s="40">
+        <v>212.8</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1994</v>
+      </c>
+      <c r="H21">
+        <f>C21+E21</f>
+        <v>403</v>
+      </c>
+      <c r="I21" s="7">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="14">
+        <v>1995</v>
+      </c>
+      <c r="C22" s="15">
+        <v>226</v>
+      </c>
+      <c r="D22" s="38">
+        <v>146.9</v>
+      </c>
+      <c r="E22" s="15">
+        <v>235</v>
+      </c>
+      <c r="F22" s="41">
+        <v>176.25</v>
+      </c>
+      <c r="G22" s="14">
+        <v>1995</v>
+      </c>
+      <c r="H22">
+        <f>C22+E22</f>
+        <v>461</v>
+      </c>
+      <c r="I22" s="15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="6">
+        <v>1996</v>
+      </c>
+      <c r="C23" s="7">
+        <v>321</v>
+      </c>
+      <c r="D23" s="37">
+        <v>138.03</v>
+      </c>
+      <c r="E23" s="7">
+        <v>355</v>
+      </c>
+      <c r="F23" s="40">
+        <v>262.7</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1996</v>
+      </c>
+      <c r="H23">
+        <f>C23+E23</f>
+        <v>676</v>
+      </c>
+      <c r="I23" s="7">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="14">
+        <v>1997</v>
+      </c>
+      <c r="C24" s="15">
+        <v>194</v>
+      </c>
+      <c r="D24" s="38">
+        <v>89.24</v>
+      </c>
+      <c r="E24" s="15">
+        <v>280</v>
+      </c>
+      <c r="F24" s="41">
+        <v>212.8</v>
+      </c>
+      <c r="G24" s="14">
+        <v>1997</v>
+      </c>
+      <c r="H24">
+        <f>C24+E24</f>
+        <v>474</v>
+      </c>
+      <c r="I24" s="15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="6">
+        <v>1998</v>
+      </c>
+      <c r="C25" s="7">
+        <v>125</v>
+      </c>
+      <c r="D25" s="37">
+        <v>46.25</v>
+      </c>
+      <c r="E25" s="7">
+        <v>156</v>
+      </c>
+      <c r="F25" s="40">
+        <v>107.64</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1998</v>
+      </c>
+      <c r="H25">
+        <f>C25+E25</f>
+        <v>281</v>
+      </c>
+      <c r="I25" s="7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="14">
+        <v>1999</v>
+      </c>
+      <c r="C26" s="15">
+        <v>382</v>
+      </c>
+      <c r="D26" s="38">
+        <v>53.48</v>
+      </c>
+      <c r="E26" s="15">
+        <v>95</v>
+      </c>
+      <c r="F26" s="41">
+        <v>59.85</v>
+      </c>
+      <c r="G26" s="14">
+        <v>1999</v>
+      </c>
+      <c r="H26">
+        <f>C26+E26</f>
+        <v>477</v>
+      </c>
+      <c r="I26" s="15">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="6">
+        <v>2000</v>
+      </c>
+      <c r="C27" s="7">
+        <v>317</v>
+      </c>
+      <c r="D27" s="37">
+        <v>41.21</v>
+      </c>
+      <c r="E27" s="7">
+        <v>64</v>
+      </c>
+      <c r="F27" s="40">
+        <v>32</v>
+      </c>
+      <c r="G27" s="6">
+        <v>2000</v>
+      </c>
+      <c r="H27">
+        <f>C27+E27</f>
+        <v>381</v>
+      </c>
+      <c r="I27" s="7">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="14">
+        <v>2001</v>
+      </c>
+      <c r="C28" s="15">
+        <v>29</v>
+      </c>
+      <c r="D28" s="38">
+        <v>6.96</v>
+      </c>
+      <c r="E28" s="15">
+        <v>50</v>
+      </c>
+      <c r="F28" s="41">
+        <v>33</v>
+      </c>
+      <c r="G28" s="14">
+        <v>2001</v>
+      </c>
+      <c r="H28">
+        <f>C28+E28</f>
+        <v>79</v>
+      </c>
+      <c r="I28" s="15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="6">
+        <v>2002</v>
+      </c>
+      <c r="C29" s="7">
+        <v>25</v>
+      </c>
+      <c r="D29" s="37">
+        <v>10.5</v>
+      </c>
+      <c r="E29" s="7">
+        <v>41</v>
+      </c>
+      <c r="F29" s="40">
+        <v>25.83</v>
+      </c>
+      <c r="G29" s="6">
+        <v>2002</v>
+      </c>
+      <c r="H29">
+        <f>C29+E29</f>
+        <v>66</v>
+      </c>
+      <c r="I29" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="14">
+        <v>2003</v>
+      </c>
+      <c r="C30" s="15">
+        <v>26</v>
+      </c>
+      <c r="D30" s="38">
+        <v>7.02</v>
+      </c>
+      <c r="E30" s="15">
+        <v>37</v>
+      </c>
+      <c r="F30" s="41">
+        <v>28.12</v>
+      </c>
+      <c r="G30" s="14">
+        <v>2003</v>
+      </c>
+      <c r="H30">
+        <f>C30+E30</f>
+        <v>63</v>
+      </c>
+      <c r="I30" s="15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="6">
+        <v>2004</v>
+      </c>
+      <c r="C31" s="7">
+        <v>91</v>
+      </c>
+      <c r="D31" s="37">
+        <v>29.12</v>
+      </c>
+      <c r="E31" s="7">
+        <v>82</v>
+      </c>
+      <c r="F31" s="40">
+        <v>57.4</v>
+      </c>
+      <c r="G31" s="6">
+        <v>2004</v>
+      </c>
+      <c r="H31">
+        <f>C31+E31</f>
+        <v>173</v>
+      </c>
+      <c r="I31" s="7">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="14">
+        <v>2005</v>
+      </c>
+      <c r="C32" s="15">
+        <v>61</v>
+      </c>
+      <c r="D32" s="38">
+        <v>18.3</v>
+      </c>
+      <c r="E32" s="15">
+        <v>98</v>
+      </c>
+      <c r="F32" s="41">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="G32" s="14">
+        <v>2005</v>
+      </c>
+      <c r="H32">
+        <f>C32+E32</f>
+        <v>159</v>
+      </c>
+      <c r="I32" s="15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="6">
+        <v>2006</v>
+      </c>
+      <c r="C33" s="7">
+        <v>72</v>
+      </c>
+      <c r="D33" s="37">
+        <v>25.92</v>
+      </c>
+      <c r="E33" s="7">
+        <v>85</v>
+      </c>
+      <c r="F33" s="40">
+        <v>68</v>
+      </c>
+      <c r="G33" s="6">
+        <v>2006</v>
+      </c>
+      <c r="H33">
+        <f>C33+E33</f>
+        <v>157</v>
+      </c>
+      <c r="I33" s="7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="14">
+        <v>2007</v>
+      </c>
+      <c r="C34" s="15">
+        <v>94</v>
+      </c>
+      <c r="D34" s="38">
+        <v>22.56</v>
+      </c>
+      <c r="E34" s="15">
+        <v>65</v>
+      </c>
+      <c r="F34" s="41">
+        <v>48.1</v>
+      </c>
+      <c r="G34" s="14">
+        <v>2007</v>
+      </c>
+      <c r="H34">
+        <f>C34+E34</f>
+        <v>159</v>
+      </c>
+      <c r="I34" s="15">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="6">
+        <v>2008</v>
+      </c>
+      <c r="C35" s="7">
+        <v>7</v>
+      </c>
+      <c r="D35" s="37">
+        <v>3.99</v>
+      </c>
+      <c r="E35" s="7">
+        <v>14</v>
+      </c>
+      <c r="F35" s="40">
+        <v>7.98</v>
+      </c>
+      <c r="G35" s="6">
+        <v>2008</v>
+      </c>
+      <c r="H35">
+        <f>C35+E35</f>
+        <v>21</v>
+      </c>
+      <c r="I35" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="14">
+        <v>2009</v>
+      </c>
+      <c r="C36" s="15">
+        <v>17</v>
+      </c>
+      <c r="D36" s="38">
+        <v>11.9</v>
+      </c>
+      <c r="E36" s="15">
+        <v>24</v>
+      </c>
+      <c r="F36" s="41">
+        <v>17.04</v>
+      </c>
+      <c r="G36" s="14">
+        <v>2009</v>
+      </c>
+      <c r="H36">
+        <f>C36+E36</f>
+        <v>41</v>
+      </c>
+      <c r="I36" s="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="6">
+        <v>2010</v>
+      </c>
+      <c r="C37" s="7">
+        <v>44</v>
+      </c>
+      <c r="D37" s="37">
+        <v>21.12</v>
+      </c>
+      <c r="E37" s="7">
+        <v>47</v>
+      </c>
+      <c r="F37" s="40">
+        <v>33.369999999999997</v>
+      </c>
+      <c r="G37" s="6">
+        <v>2010</v>
+      </c>
+      <c r="H37">
+        <f>C37+E37</f>
+        <v>91</v>
+      </c>
+      <c r="I37" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="14">
+        <v>2011</v>
+      </c>
+      <c r="C38" s="15">
+        <v>44</v>
+      </c>
+      <c r="D38" s="38">
+        <v>12.76</v>
+      </c>
+      <c r="E38" s="15">
+        <v>37</v>
+      </c>
+      <c r="F38" s="41">
+        <v>22.2</v>
+      </c>
+      <c r="G38" s="14">
+        <v>2011</v>
+      </c>
+      <c r="H38">
+        <f>C38+E38</f>
+        <v>81</v>
+      </c>
+      <c r="I38" s="15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C39" s="7">
+        <v>49</v>
+      </c>
+      <c r="D39" s="37">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="E39" s="7">
+        <v>44</v>
+      </c>
+      <c r="F39" s="40">
+        <v>33</v>
+      </c>
+      <c r="G39" s="6">
+        <v>2012</v>
+      </c>
+      <c r="H39">
+        <f>C39+E39</f>
+        <v>93</v>
+      </c>
+      <c r="I39" s="7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="14">
+        <v>2013</v>
+      </c>
+      <c r="C40" s="15">
+        <v>84</v>
+      </c>
+      <c r="D40" s="38">
+        <v>15.96</v>
+      </c>
+      <c r="E40" s="15">
+        <v>73</v>
+      </c>
+      <c r="F40" s="41">
+        <v>40.880000000000003</v>
+      </c>
+      <c r="G40" s="14">
+        <v>2013</v>
+      </c>
+      <c r="H40">
+        <f>C40+E40</f>
+        <v>157</v>
+      </c>
+      <c r="I40" s="15">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="10">
+        <v>2014</v>
+      </c>
+      <c r="C41" s="11">
+        <v>127</v>
+      </c>
+      <c r="D41" s="39">
+        <v>13.97</v>
+      </c>
+      <c r="E41" s="11">
+        <v>79</v>
+      </c>
+      <c r="F41" s="42">
+        <v>45.03</v>
+      </c>
+      <c r="G41" s="10">
+        <v>2014</v>
+      </c>
+      <c r="H41">
+        <f>C41+E41</f>
+        <v>206</v>
+      </c>
+      <c r="I41" s="11">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
@@ -786,7 +1928,7 @@
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6">
       <c r="B5" s="2"/>
       <c r="C5" s="35" t="s">
         <v>2</v>
@@ -797,7 +1939,7 @@
       </c>
       <c r="F5" s="36"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -814,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6">
       <c r="B7" s="6">
         <v>1980</v>
       </c>
@@ -831,7 +1973,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6">
       <c r="B8" s="14">
         <v>1981</v>
       </c>
@@ -848,7 +1990,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6">
       <c r="B9" s="6">
         <v>1982</v>
       </c>
@@ -865,7 +2007,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6">
       <c r="B10" s="14">
         <v>1983</v>
       </c>
@@ -882,7 +2024,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6">
       <c r="B11" s="6">
         <v>1984</v>
       </c>
@@ -899,7 +2041,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6">
       <c r="B12" s="14">
         <v>1985</v>
       </c>
@@ -916,7 +2058,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6">
       <c r="B13" s="6">
         <v>1986</v>
       </c>
@@ -933,7 +2075,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6">
       <c r="B14" s="14">
         <v>1987</v>
       </c>
@@ -950,7 +2092,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6">
       <c r="B15" s="6">
         <v>1988</v>
       </c>
@@ -967,7 +2109,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6">
       <c r="B16" s="14">
         <v>1989</v>
       </c>
@@ -984,7 +2126,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6">
       <c r="B17" s="6">
         <v>1990</v>
       </c>
@@ -1001,7 +2143,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6">
       <c r="B18" s="14">
         <v>1991</v>
       </c>
@@ -1018,7 +2160,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6">
       <c r="B19" s="6">
         <v>1992</v>
       </c>
@@ -1035,7 +2177,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6">
       <c r="B20" s="14">
         <v>1993</v>
       </c>
@@ -1052,7 +2194,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6">
       <c r="B21" s="6">
         <v>1994</v>
       </c>
@@ -1069,7 +2211,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6">
       <c r="B22" s="14">
         <v>1995</v>
       </c>
@@ -1086,7 +2228,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6">
       <c r="B23" s="6">
         <v>1996</v>
       </c>
@@ -1103,7 +2245,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6">
       <c r="B24" s="14">
         <v>1997</v>
       </c>
@@ -1120,7 +2262,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6">
       <c r="B25" s="6">
         <v>1998</v>
       </c>
@@ -1137,7 +2279,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6">
       <c r="B26" s="14">
         <v>1999</v>
       </c>
@@ -1154,7 +2296,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6">
       <c r="B27" s="6">
         <v>2000</v>
       </c>
@@ -1171,7 +2313,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6">
       <c r="B28" s="14">
         <v>2001</v>
       </c>
@@ -1188,7 +2330,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6">
       <c r="B29" s="6">
         <v>2002</v>
       </c>
@@ -1205,7 +2347,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6">
       <c r="B30" s="14">
         <v>2003</v>
       </c>
@@ -1222,7 +2364,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6">
       <c r="B31" s="6">
         <v>2004</v>
       </c>
@@ -1239,7 +2381,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6">
       <c r="B32" s="14">
         <v>2005</v>
       </c>
@@ -1256,7 +2398,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6">
       <c r="B33" s="6">
         <v>2006</v>
       </c>
@@ -1273,7 +2415,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6">
       <c r="B34" s="14">
         <v>2007</v>
       </c>
@@ -1290,7 +2432,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6">
       <c r="B35" s="6">
         <v>2008</v>
       </c>
@@ -1307,7 +2449,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6">
       <c r="B36" s="14">
         <v>2009</v>
       </c>
@@ -1324,7 +2466,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6">
       <c r="B37" s="6">
         <v>2010</v>
       </c>
@@ -1341,7 +2483,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6">
       <c r="B38" s="14">
         <v>2011</v>
       </c>
@@ -1358,7 +2500,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6">
       <c r="B39" s="6">
         <v>2012</v>
       </c>
@@ -1375,7 +2517,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6">
       <c r="B40" s="14">
         <v>2013</v>
       </c>
@@ -1392,7 +2534,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6">
       <c r="B41" s="10">
         <v>2014</v>
       </c>
@@ -1416,10 +2558,15 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G21"/>
   <sheetViews>
@@ -1427,14 +2574,14 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="7" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" ht="13" customHeight="1"/>
+    <row r="6" spans="2:7">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1444,7 +2591,7 @@
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7">
       <c r="B7" s="18" t="s">
         <v>10</v>
       </c>
@@ -1464,7 +2611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7">
       <c r="B8" s="19" t="s">
         <v>5</v>
       </c>
@@ -1484,7 +2631,7 @@
         <v>0.20349999999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7">
       <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
@@ -1504,7 +2651,7 @@
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +2661,7 @@
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7">
       <c r="B12" s="18" t="s">
         <v>10</v>
       </c>
@@ -1534,7 +2681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7">
       <c r="B13" s="19" t="s">
         <v>5</v>
       </c>
@@ -1554,7 +2701,7 @@
         <v>3.5099999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7">
       <c r="B14" s="21" t="s">
         <v>18</v>
       </c>
@@ -1574,7 +2721,7 @@
         <v>9.7600000000000006E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7">
       <c r="B15" s="20" t="s">
         <v>8</v>
       </c>
@@ -1594,7 +2741,7 @@
         <v>3.1300000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7">
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1604,7 +2751,7 @@
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7">
       <c r="B18" s="18" t="s">
         <v>10</v>
       </c>
@@ -1624,7 +2771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7">
       <c r="B19" s="19" t="s">
         <v>6</v>
       </c>
@@ -1644,7 +2791,7 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7">
       <c r="B20" s="21" t="s">
         <v>17</v>
       </c>
@@ -1664,7 +2811,7 @@
         <v>1.5100000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7">
       <c r="B21" s="20" t="s">
         <v>5</v>
       </c>
@@ -1687,5 +2834,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>